<commit_message>
deliver task 3 arm sprint commit 2
</commit_message>
<xml_diff>
--- a/07_Sprint_Twelve/02_RGB_LED_CONTROL_V2.0/01_Documentation/00_pdfs/Team Backlog.xlsx
+++ b/07_Sprint_Twelve/02_RGB_LED_CONTROL_V2.0/01_Documentation/00_pdfs/Team Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Embedded System Diploma\Sprints\sprints_github\SPRINTS_Automotive_Software_Bootcamp\07_Sprint_Twelve\01_RGB_LED_CONTROL_V1.0\01_Documentation\00_pdfs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programing\Embedded System Diploma\Sprints\sprints_github\SPRINTS_Automotive_Software_Bootcamp\07_Sprint_Twelve\02_RGB_LED_CONTROL_V2.0\01_Documentation\00_pdfs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E31C40B-D457-4FA5-AFE7-134C5C28DBCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF0532D-9FDB-4BA7-99A3-6F0CCBA7D38B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{875C6DCD-AFAF-4A5F-9F21-083CA0FCED6F}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
   <si>
     <t>Task Name</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>4 hour</t>
+  </si>
+  <si>
+    <t>SYSTICK_init</t>
+  </si>
+  <si>
+    <t>SYSTICK_interruptEnable</t>
+  </si>
+  <si>
+    <t>SYSTICK_interruptDisable</t>
+  </si>
+  <si>
+    <t>SYSTICK_setDelayInMs</t>
+  </si>
+  <si>
+    <t>SYSTICK_handler</t>
   </si>
 </sst>
 </file>
@@ -528,7 +543,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C123E326-AE56-4BD1-BFE1-3D77BAFFAE7E}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
@@ -807,19 +822,19 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="D14" s="1">
         <v>100</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -827,19 +842,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="D15" s="1">
         <v>100</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>31</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -847,24 +862,124 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="1">
+        <v>100</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="1">
+        <v>100</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="1">
+        <v>100</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19" s="1">
+        <v>100</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1">
+        <v>100</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="1">
-        <v>100</v>
-      </c>
-      <c r="E16" s="5" t="s">
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1">
+        <v>100</v>
+      </c>
+      <c r="E21" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F21" s="5" t="s">
         <v>32</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
-  <conditionalFormatting sqref="D2:D51">
+  <conditionalFormatting sqref="D2:D56">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="min"/>
@@ -892,7 +1007,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>D2:D51</xm:sqref>
+          <xm:sqref>D2:D56</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>